<commit_message>
Criada a classe ar condicionado e corrigidos problemas com a classe planilha
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -427,9 +427,48 @@
         </is>
       </c>
       <c r="B1" t="n">
-        <v>70</v>
+        <v>100</v>
       </c>
       <c r="C1" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Lampada da sala</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Ar da sala</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>18</v>
+      </c>
+      <c r="C3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Ar do quarto</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>23</v>
+      </c>
+      <c r="C4" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionando classe televisao e realizando testes
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -430,45 +430,6 @@
         <v>100</v>
       </c>
       <c r="C1" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Lampada da sala</t>
-        </is>
-      </c>
-      <c r="B2" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Ar da sala</t>
-        </is>
-      </c>
-      <c r="B3" t="n">
-        <v>18</v>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Ar do quarto</t>
-        </is>
-      </c>
-      <c r="B4" t="n">
-        <v>23</v>
-      </c>
-      <c r="C4" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
correção na classe planilha
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -16,13 +16,25 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -33,7 +45,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -43,10 +62,37 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,27 +458,105 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="4" max="4"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="7" t="inlineStr">
         <is>
           <t>Lampada do quarto</t>
         </is>
       </c>
-      <c r="B1" t="n">
+      <c r="B1" s="4" t="n">
         <v>100</v>
       </c>
-      <c r="C1" t="b">
-        <v>0</v>
-      </c>
+      <c r="C1" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7" t="n"/>
     </row>
+    <row r="2" ht="19.5" customHeight="1">
+      <c r="A2" s="7" t="inlineStr">
+        <is>
+          <t>Ar da sala</t>
+        </is>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>18</v>
+      </c>
+      <c r="C2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="n"/>
+    </row>
+    <row r="3" ht="19.5" customHeight="1">
+      <c r="A3" s="7" t="inlineStr">
+        <is>
+          <t>Tv do quarto</t>
+        </is>
+      </c>
+      <c r="B3" s="5" t="n"/>
+      <c r="C3" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D3" s="7" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+    </row>
+    <row r="4" ht="19.5" customHeight="1">
+      <c r="A4" s="7" t="inlineStr">
+        <is>
+          <t>Tv da sala</t>
+        </is>
+      </c>
+      <c r="B4" s="6" t="inlineStr">
+        <is>
+          <t>Canal 3</t>
+        </is>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="D4" s="7" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+    </row>
+    <row r="5" ht="19.5" customHeight="1">
+      <c r="A5" s="7" t="inlineStr">
+        <is>
+          <t>Tv da cozinha</t>
+        </is>
+      </c>
+      <c r="B5" s="8" t="inlineStr">
+        <is>
+          <t>Canal 3</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>10</v>
+      </c>
+      <c r="D5" s="7" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="18.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
criado o objeto caixa de som
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -64,22 +64,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left"/>
@@ -458,7 +452,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -466,97 +460,117 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="9" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="7" t="inlineStr">
+    <row r="1" ht="19.5" customHeight="1">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Lampada do quarto</t>
         </is>
       </c>
-      <c r="B1" s="4" t="n">
+      <c r="B1" s="2" t="n">
         <v>100</v>
       </c>
-      <c r="C1" s="5" t="b">
+      <c r="C1" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D1" s="7" t="n"/>
+      <c r="D1" s="5" t="n"/>
     </row>
     <row r="2" ht="19.5" customHeight="1">
-      <c r="A2" s="7" t="inlineStr">
+      <c r="A2" s="5" t="inlineStr">
         <is>
           <t>Ar da sala</t>
         </is>
       </c>
-      <c r="B2" s="4" t="n">
+      <c r="B2" s="2" t="n">
         <v>18</v>
       </c>
-      <c r="C2" s="5" t="b">
+      <c r="C2" s="2" t="b">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="n"/>
+      <c r="D2" s="5" t="n"/>
     </row>
     <row r="3" ht="19.5" customHeight="1">
-      <c r="A3" s="7" t="inlineStr">
+      <c r="A3" s="5" t="inlineStr">
         <is>
           <t>Tv do quarto</t>
         </is>
       </c>
-      <c r="B3" s="5" t="n"/>
-      <c r="C3" s="4" t="n">
+      <c r="B3" s="2" t="n"/>
+      <c r="C3" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D3" s="7" t="inlineStr">
+      <c r="D3" s="5" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
     </row>
     <row r="4" ht="19.5" customHeight="1">
-      <c r="A4" s="7" t="inlineStr">
+      <c r="A4" s="5" t="inlineStr">
         <is>
           <t>Tv da sala</t>
         </is>
       </c>
-      <c r="B4" s="6" t="inlineStr">
+      <c r="B4" s="3" t="inlineStr">
         <is>
           <t>Canal 3</t>
         </is>
       </c>
-      <c r="C4" s="4" t="n">
+      <c r="C4" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D4" s="7" t="inlineStr">
+      <c r="D4" s="5" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
     </row>
     <row r="5" ht="19.5" customHeight="1">
-      <c r="A5" s="7" t="inlineStr">
+      <c r="A5" s="5" t="inlineStr">
         <is>
           <t>Tv da cozinha</t>
         </is>
       </c>
-      <c r="B5" s="8" t="inlineStr">
+      <c r="B5" s="4" t="inlineStr">
         <is>
           <t>Canal 3</t>
         </is>
       </c>
-      <c r="C5" s="5" t="n">
+      <c r="C5" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="D5" s="7" t="inlineStr">
+      <c r="D5" s="5" t="inlineStr">
         <is>
           <t>true</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="18.75" customHeight="1"/>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Alexa</t>
+        </is>
+      </c>
+      <c r="B6" t="b">
+        <v>0</v>
+      </c>
+      <c r="C6" t="n">
+        <v>50</v>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Leo Santana</t>
+        </is>
+      </c>
+      <c r="E6" t="b">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modificação na função salvar
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -1,45 +1,62 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+  <si>
+    <t>Ar da sala</t>
+  </si>
+  <si>
+    <t>Alexa</t>
+  </si>
+  <si>
+    <t>Leo Santana</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>Tv da cozinha</t>
+  </si>
+  <si>
+    <t>Canal 3</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="11"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -62,104 +79,42 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -447,129 +402,67 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19.5" customHeight="1">
-      <c r="A1" s="5" t="inlineStr">
-        <is>
-          <t>Lampada do quarto</t>
-        </is>
-      </c>
-      <c r="B1" s="2" t="n">
-        <v>100</v>
-      </c>
-      <c r="C1" s="2" t="b">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2">
+        <v>18</v>
+      </c>
+      <c r="C1" s="3" t="b">
         <v>1</v>
       </c>
-      <c r="D1" s="5" t="n"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
     </row>
-    <row r="2" ht="19.5" customHeight="1">
-      <c r="A2" s="5" t="inlineStr">
-        <is>
-          <t>Ar da sala</t>
-        </is>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>18</v>
-      </c>
-      <c r="C2" s="2" t="b">
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5" t="n"/>
+      <c r="B2" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2">
+        <v>50</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" ht="19.5" customHeight="1">
-      <c r="A3" s="5" t="inlineStr">
-        <is>
-          <t>Tv do quarto</t>
-        </is>
-      </c>
-      <c r="B3" s="2" t="n"/>
-      <c r="C3" s="2" t="n">
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2">
         <v>10</v>
       </c>
-      <c r="D3" s="5" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="19.5" customHeight="1">
-      <c r="A4" s="5" t="inlineStr">
-        <is>
-          <t>Tv da sala</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>Canal 3</t>
-        </is>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="D4" s="5" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-    </row>
-    <row r="5" ht="19.5" customHeight="1">
-      <c r="A5" s="5" t="inlineStr">
-        <is>
-          <t>Tv da cozinha</t>
-        </is>
-      </c>
-      <c r="B5" s="4" t="inlineStr">
-        <is>
-          <t>Canal 3</t>
-        </is>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="D5" s="5" t="inlineStr">
-        <is>
-          <t>true</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Alexa</t>
-        </is>
-      </c>
-      <c r="B6" t="b">
-        <v>0</v>
-      </c>
-      <c r="C6" t="n">
-        <v>50</v>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Leo Santana</t>
-        </is>
-      </c>
-      <c r="E6" t="b">
-        <v>1</v>
-      </c>
+      <c r="D3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Correções na classe planilha
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -1,62 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
-  <si>
-    <t>Ar da sala</t>
-  </si>
-  <si>
-    <t>Alexa</t>
-  </si>
-  <si>
-    <t>Leo Santana</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>Tv da cozinha</t>
-  </si>
-  <si>
-    <t>Canal 3</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -79,42 +56,107 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+  <cellXfs count="9">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -402,67 +444,104 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="4" max="4"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
+    <row r="1" ht="18.75" customHeight="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>Lampada do quarto</t>
+        </is>
+      </c>
+      <c r="B1" s="6" t="inlineStr">
+        <is>
+          <t>lampada</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="D1" s="8" t="b">
         <v>0</v>
       </c>
-      <c r="B1" s="2">
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Ar da sala</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>climatizadores</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
         <v>18</v>
       </c>
-      <c r="C1" s="3" t="b">
+      <c r="D2" t="b">
         <v>1</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="1" t="s">
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Alexa</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>alto falante</t>
+        </is>
+      </c>
+      <c r="C3" t="b">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="b">
+      <c r="D3" t="n">
+        <v>50</v>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Leo Santana</t>
+        </is>
+      </c>
+      <c r="F3" t="b">
         <v>1</v>
       </c>
-      <c r="C2" s="2">
-        <v>50</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="2">
-        <v>10</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1"/>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Lampada da sala</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>lampada</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Base do 'adicionar novo dispositivo'
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -543,6 +543,57 @@
         <v>0</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Tv da cozinha</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Canal 3</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>10</v>
+      </c>
+      <c r="D5" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Fechadura dos fundos</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>fechadura</t>
+        </is>
+      </c>
+      <c r="C6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Ar do banheiro</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>climatizadores</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>23</v>
+      </c>
+      <c r="D7" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
base para interface dos dispositivos
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -455,7 +455,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
     <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
@@ -478,7 +478,7 @@
         <v>100</v>
       </c>
       <c r="D1" s="8" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2">
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="C3" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D3" t="n">
         <v>50</v>
@@ -558,7 +558,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
correções na base da interface
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -478,7 +478,7 @@
         <v>100</v>
       </c>
       <c r="D1" s="8" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2">
@@ -511,7 +511,7 @@
         </is>
       </c>
       <c r="C3" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" t="n">
         <v>50</v>
@@ -558,7 +558,7 @@
         <v>10</v>
       </c>
       <c r="D5" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">

</xml_diff>

<commit_message>
Correção da TV na planilha
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -449,7 +449,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -643,6 +643,24 @@
         <v>0</v>
       </c>
     </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>TV do banheiro</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>televisao</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
correçao de erros na hora de salvar, implementação de mensagens de erro e confirmação
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -27,7 +27,7 @@
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
+      <color rgb="FF000000"/>
       <sz val="11"/>
     </font>
   </fonts>
@@ -58,31 +58,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
+      <alignment horizontal="general"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="general"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -449,7 +440,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -457,207 +448,361 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="7" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="8" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="4" max="4"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="3" min="5" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="5" t="inlineStr">
-        <is>
-          <t>Lampada do quarto</t>
-        </is>
-      </c>
-      <c r="B1" s="6" t="inlineStr">
-        <is>
-          <t>lampada</t>
-        </is>
-      </c>
-      <c r="C1" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="D1" s="8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Ar da sala</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>climatizadores</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>18</v>
-      </c>
-      <c r="D2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Alexa</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>alto falante</t>
-        </is>
-      </c>
-      <c r="C3" t="b">
-        <v>1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>50</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Leo Santana</t>
-        </is>
-      </c>
-      <c r="F3" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Lampada da sala</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>lampada</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Tv da cozinha</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Canal 3</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>10</v>
-      </c>
-      <c r="D5" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Fechadura dos fundos</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>fechadura</t>
-        </is>
-      </c>
-      <c r="C6" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Ar do banheiro</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>climatizadores</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
+    <row r="1" ht="19.5" customHeight="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>ar1</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="D7" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>ac 1</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>climatizadores</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
+      <c r="D1" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E1" s="3" t="n"/>
+    </row>
+    <row r="2" ht="19.5" customHeight="1">
+      <c r="A2" s="3" t="inlineStr">
+        <is>
+          <t>ar2</t>
+        </is>
+      </c>
+      <c r="B2" s="3" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="n">
         <v>23</v>
       </c>
-      <c r="D8" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>lamp 2</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>lampada</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>tv 3</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
-      <c r="D10" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>TV do banheiro</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>televisao</t>
-        </is>
-      </c>
-      <c r="D11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E11" t="b">
+      <c r="D2" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="n"/>
+    </row>
+    <row r="3" ht="19.5" customHeight="1">
+      <c r="A3" s="3" t="inlineStr">
+        <is>
+          <t>ar3</t>
+        </is>
+      </c>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="C3" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="n"/>
+    </row>
+    <row r="4" ht="19.5" customHeight="1">
+      <c r="A4" s="3" t="inlineStr">
+        <is>
+          <t>ar4</t>
+        </is>
+      </c>
+      <c r="B4" s="3" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="n"/>
+    </row>
+    <row r="5" ht="19.5" customHeight="1">
+      <c r="A5" s="3" t="inlineStr">
+        <is>
+          <t>ar5</t>
+        </is>
+      </c>
+      <c r="B5" s="3" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="n"/>
+    </row>
+    <row r="6" ht="19.5" customHeight="1">
+      <c r="A6" s="3" t="inlineStr">
+        <is>
+          <t>ar6</t>
+        </is>
+      </c>
+      <c r="B6" s="3" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>23</v>
+      </c>
+      <c r="D6" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3" t="n"/>
+    </row>
+    <row r="7" ht="19.5" customHeight="1">
+      <c r="A7" s="3" t="inlineStr">
+        <is>
+          <t>L1</t>
+        </is>
+      </c>
+      <c r="B7" s="3" t="inlineStr">
+        <is>
+          <t>Lâmpada</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3" t="n"/>
+    </row>
+    <row r="8" ht="19.5" customHeight="1">
+      <c r="A8" s="3" t="inlineStr">
+        <is>
+          <t>L2</t>
+        </is>
+      </c>
+      <c r="B8" s="3" t="inlineStr">
+        <is>
+          <t>Lâmpada</t>
+        </is>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3" t="n"/>
+    </row>
+    <row r="9" ht="19.5" customHeight="1">
+      <c r="A9" s="3" t="inlineStr">
+        <is>
+          <t>L3</t>
+        </is>
+      </c>
+      <c r="B9" s="3" t="inlineStr">
+        <is>
+          <t>Lâmpada</t>
+        </is>
+      </c>
+      <c r="C9" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E9" s="3" t="n"/>
+    </row>
+    <row r="10" ht="19.5" customHeight="1">
+      <c r="A10" s="3" t="inlineStr">
+        <is>
+          <t>L4</t>
+        </is>
+      </c>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>Lâmpada</t>
+        </is>
+      </c>
+      <c r="C10" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D10" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E10" s="3" t="n"/>
+    </row>
+    <row r="11" ht="19.5" customHeight="1">
+      <c r="A11" s="3" t="inlineStr">
+        <is>
+          <t>L5</t>
+        </is>
+      </c>
+      <c r="B11" s="3" t="inlineStr">
+        <is>
+          <t>Lâmpada</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D11" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E11" s="3" t="n"/>
+    </row>
+    <row r="12" ht="19.5" customHeight="1">
+      <c r="A12" s="3" t="inlineStr">
+        <is>
+          <t>L6</t>
+        </is>
+      </c>
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>Lâmpada</t>
+        </is>
+      </c>
+      <c r="C12" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D12" s="2" t="b">
+        <v>0</v>
+      </c>
+      <c r="E12" s="3" t="n"/>
+    </row>
+    <row r="13" ht="19.5" customHeight="1">
+      <c r="A13" s="3" t="inlineStr">
+        <is>
+          <t>tv1</t>
+        </is>
+      </c>
+      <c r="B13" s="3" t="inlineStr">
+        <is>
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="C13" s="2" t="n"/>
+      <c r="D13" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E13" s="3" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+    </row>
+    <row r="14" ht="19.5" customHeight="1">
+      <c r="A14" s="3" t="inlineStr">
+        <is>
+          <t>tv2</t>
+        </is>
+      </c>
+      <c r="B14" s="3" t="inlineStr">
+        <is>
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="C14" s="2" t="n"/>
+      <c r="D14" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E14" s="3" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+    </row>
+    <row r="15" ht="19.5" customHeight="1">
+      <c r="A15" s="3" t="inlineStr">
+        <is>
+          <t>tv3</t>
+        </is>
+      </c>
+      <c r="B15" s="3" t="inlineStr">
+        <is>
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="C15" s="2" t="n"/>
+      <c r="D15" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E15" s="3" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+    </row>
+    <row r="16" ht="19.5" customHeight="1">
+      <c r="A16" s="3" t="inlineStr">
+        <is>
+          <t>tv4</t>
+        </is>
+      </c>
+      <c r="B16" s="3" t="inlineStr">
+        <is>
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="C16" s="2" t="n"/>
+      <c r="D16" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E16" s="3" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+    </row>
+    <row r="17" ht="19.5" customHeight="1">
+      <c r="A17" s="3" t="inlineStr">
+        <is>
+          <t>tv5</t>
+        </is>
+      </c>
+      <c r="B17" s="3" t="inlineStr">
+        <is>
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="C17" s="2" t="n"/>
+      <c r="D17" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E17" s="3" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>tv</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrigindo erro de lógica do mesmo nome do disp
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -1,37 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -50,18 +46,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -349,16 +407,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
+    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="C1" t="n">
+        <v>23</v>
+      </c>
+      <c r="D1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>teste</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>23</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>new ar</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>23</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>lamp1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Lâmpada</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ajustando posicoes dos botoes e dos textos
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -45,8 +45,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,18 +421,24 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="12.43357142857143" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
+    <col width="12.43357142857143" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="12.43357142857143" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
+    <col width="12.43357142857143" bestFit="1" customWidth="1" style="3" min="4" max="4"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>teste</t>
+          <t>Teste</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -441,54 +456,18 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>teste</t>
+          <t>Tv da sala</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>A/C</t>
+          <t>Televisor</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>23</v>
-      </c>
-      <c r="D2" t="b">
+      <c r="D2" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>new ar</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>A/C</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>23</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>lamp1</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Lâmpada</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D4" t="b">
+      <c r="E2" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adicionada a função de remover dispositivo
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -45,17 +45,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,24 +412,18 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="12.43357142857143" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
-    <col width="12.43357142857143" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
-    <col width="12.43357142857143" bestFit="1" customWidth="1" style="2" min="3" max="3"/>
-    <col width="12.43357142857143" bestFit="1" customWidth="1" style="3" min="4" max="4"/>
-  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Teste</t>
+          <t>Ar da sala</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -453,24 +438,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Tv da sala</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Televisor</t>
-        </is>
-      </c>
-      <c r="D2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" t="b">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
implementação da interface AC, modificações no botao dinamico
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -427,7 +427,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
     <col width="12.43357142857143" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
     <col width="12.43357142857143" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
@@ -447,7 +447,7 @@
         </is>
       </c>
       <c r="C1" t="n">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D1" t="b">
         <v>0</v>

</xml_diff>

<commit_message>
melhorias na interface ac
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -446,7 +446,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,45 +464,49 @@
     <row r="1" ht="18.75" customHeight="1">
       <c r="A1" s="5" t="inlineStr">
         <is>
-          <t>Ar da sala</t>
+          <t>TV da sala</t>
         </is>
       </c>
       <c r="B1" s="5" t="inlineStr">
         <is>
-          <t>A/C</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="n">
-        <v>23</v>
-      </c>
-      <c r="D1" s="7" t="b">
-        <v>1</v>
-      </c>
-      <c r="E1" s="5" t="n"/>
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="n"/>
+      <c r="D1" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="18.75" customHeight="1">
       <c r="A2" s="5" t="inlineStr">
         <is>
-          <t>Ar do quarto</t>
+          <t>TV da cozinha</t>
         </is>
       </c>
       <c r="B2" s="5" t="inlineStr">
         <is>
-          <t>A/C</t>
-        </is>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>23</v>
-      </c>
-      <c r="D2" s="7" t="b">
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="C2" s="6" t="n"/>
+      <c r="D2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="E2" s="5" t="n"/>
+      <c r="E2" s="5" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
     </row>
     <row r="3" ht="18.75" customHeight="1">
       <c r="A3" s="5" t="inlineStr">
         <is>
-          <t>TV da sala</t>
+          <t>TV da area</t>
         </is>
       </c>
       <c r="B3" s="5" t="inlineStr">
@@ -521,63 +525,39 @@
       </c>
     </row>
     <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" s="5" t="inlineStr">
-        <is>
-          <t>TV da cozinha</t>
-        </is>
-      </c>
-      <c r="B4" s="5" t="inlineStr">
-        <is>
-          <t>Televisor</t>
-        </is>
-      </c>
-      <c r="C4" s="6" t="n"/>
-      <c r="D4" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="5" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>ar2</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>17</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" s="5" t="inlineStr">
-        <is>
-          <t>TV da area</t>
-        </is>
-      </c>
-      <c r="B5" s="5" t="inlineStr">
-        <is>
-          <t>Televisor</t>
-        </is>
-      </c>
-      <c r="C5" s="6" t="n"/>
-      <c r="D5" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="5" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Ar1</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>ar3</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>A/C</t>
         </is>
       </c>
-      <c r="C6" t="n">
-        <v>23</v>
-      </c>
-      <c r="D6" t="b">
-        <v>0</v>
+      <c r="C5" t="n">
+        <v>30</v>
+      </c>
+      <c r="D5" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
criada a tela de inicio
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -1,52 +1,43 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Sheet1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -56,104 +47,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
+  <cellXfs count="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -441,126 +349,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
-    <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="12.43357142857143" bestFit="1" customWidth="1" style="5" min="1" max="1"/>
-    <col width="12.43357142857143" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
-    <col width="12.43357142857143" bestFit="1" customWidth="1" style="6" min="3" max="3"/>
-    <col width="12.43357142857143" bestFit="1" customWidth="1" style="7" min="4" max="4"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
-      <c r="A1" s="5" t="inlineStr">
-        <is>
-          <t>TV da sala</t>
-        </is>
-      </c>
-      <c r="B1" s="5" t="inlineStr">
-        <is>
-          <t>Televisor</t>
-        </is>
-      </c>
-      <c r="C1" s="6" t="n"/>
-      <c r="D1" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E1" s="5" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-    </row>
-    <row r="2" ht="18.75" customHeight="1">
-      <c r="A2" s="5" t="inlineStr">
-        <is>
-          <t>TV da cozinha</t>
-        </is>
-      </c>
-      <c r="B2" s="5" t="inlineStr">
-        <is>
-          <t>Televisor</t>
-        </is>
-      </c>
-      <c r="C2" s="6" t="n"/>
-      <c r="D2" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="5" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-    </row>
-    <row r="3" ht="18.75" customHeight="1">
-      <c r="A3" s="5" t="inlineStr">
-        <is>
-          <t>TV da area</t>
-        </is>
-      </c>
-      <c r="B3" s="5" t="inlineStr">
-        <is>
-          <t>Televisor</t>
-        </is>
-      </c>
-      <c r="C3" s="6" t="n"/>
-      <c r="D3" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="5" t="inlineStr">
-        <is>
-          <t>false</t>
-        </is>
-      </c>
-    </row>
-    <row r="4" ht="18.75" customHeight="1">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>ar2</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>A/C</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>17</v>
-      </c>
-      <c r="D4" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" ht="18.75" customHeight="1">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>ar3</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>A/C</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>30</v>
-      </c>
-      <c r="D5" t="b">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
criada a interface lampada
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -16,13 +16,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -33,7 +39,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -43,10 +56,28 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,29 +443,53 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
+    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="4" max="4"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="18.75" customHeight="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Ar da sala</t>
+          <t>TV da sala</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>A/C</t>
+          <t>Televisor</t>
         </is>
       </c>
-      <c r="C1" t="n">
-        <v>19</v>
-      </c>
-      <c r="D1" t="b">
+      <c r="D1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Tv da cozinha</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adicionando check botao concluir
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -443,7 +443,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -493,6 +493,24 @@
         <v>0</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ar sala</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>23</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
implementada a interface da tv e corrigidos alguns bugs
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -16,19 +16,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="1">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
@@ -39,14 +33,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -56,28 +43,10 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -443,72 +412,51 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <cols>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="1" max="1"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="4" min="2" max="2"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="5" min="3" max="3"/>
-    <col width="13.57642857142857" bestFit="1" customWidth="1" style="6" min="4" max="4"/>
-  </cols>
   <sheetData>
-    <row r="1" ht="18.75" customHeight="1">
+    <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>TV da sala</t>
+          <t>ar da sala</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Televisor</t>
+          <t>A/C</t>
         </is>
       </c>
+      <c r="C1" t="n">
+        <v>23</v>
+      </c>
       <c r="D1" t="b">
-        <v>1</v>
-      </c>
-      <c r="E1" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>lamp sala</t>
+          <t>TV da sala</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Lâmpada</t>
+          <t>Televisor</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Ar quarto</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>A/C</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>19</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
+        <v>12</v>
+      </c>
+      <c r="D2" t="n">
+        <v>36</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
melhorias na modularização e correção nas cores de fundo
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -412,54 +412,14 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>ar da sala</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>A/C</t>
-        </is>
-      </c>
-      <c r="C1" t="n">
-        <v>23</v>
-      </c>
-      <c r="D1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>TV da sala</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Televisor</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>12</v>
-      </c>
-      <c r="D2" t="n">
-        <v>36</v>
-      </c>
-      <c r="E2" t="b">
-        <v>1</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
correções nas cores de fundo dos sliders e textos
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -412,14 +412,72 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>A/C</t>
+        </is>
+      </c>
+      <c r="C1" t="n">
+        <v>23</v>
+      </c>
+      <c r="D1" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>b</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Lâmpada</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>c</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Televisor</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Comentando .src e corrigindo problema da planilha
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,57 +462,36 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>d</t>
+          <t>e</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Televisor</t>
+          <t>Lâmpada</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" t="n">
-        <v>47</v>
-      </c>
-      <c r="E3" t="b">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="D3" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>e</t>
+          <t>f</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Lâmpada</t>
+          <t>A/C</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="D4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>f</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>A/C</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>23</v>
-      </c>
-      <c r="D5" t="b">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Centralizando textos e adicionando novas mensagens de retorno
</commit_message>
<xml_diff>
--- a/objetos.xlsx
+++ b/objetos.xlsx
@@ -412,87 +412,14 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>a</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>A/C</t>
-        </is>
-      </c>
-      <c r="C1" t="n">
-        <v>26</v>
-      </c>
-      <c r="D1" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>e</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Lâmpada</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
-      <c r="D2" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>f</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>A/C</t>
-        </is>
-      </c>
-      <c r="C3" t="n">
-        <v>23</v>
-      </c>
-      <c r="D3" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>j</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>A/C</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>23</v>
-      </c>
-      <c r="D4" t="b">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>